<commit_message>
adding folder for the supplemental data
</commit_message>
<xml_diff>
--- a/TPDS/experiments/register_tile_bench_mark.xlsx
+++ b/TPDS/experiments/register_tile_bench_mark.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/MyDocuments/Techinical Documents/Masters/Thesis/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chiranjeb/alphaz-user-docker/workspace/bpmax_cpu/TPDS/experiments/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E73CECC-A6BE-D14B-A351-679701F54B4F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B77DF61E-0D64-3C47-BAAA-666DD88A011E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="840" yWindow="500" windowWidth="38920" windowHeight="21140" activeTab="2" xr2:uid="{6E17427D-3CC4-634F-B2A9-A5E44CDE0F3C}"/>
+    <workbookView xWindow="2100" yWindow="500" windowWidth="38920" windowHeight="21140" activeTab="4" xr2:uid="{6E17427D-3CC4-634F-B2A9-A5E44CDE0F3C}"/>
   </bookViews>
   <sheets>
     <sheet name="Raw Data - New" sheetId="3" r:id="rId1"/>
@@ -431,6 +431,10 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -452,10 +456,6 @@
     <xf numFmtId="0" fontId="1" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -487,15 +487,70 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
-    <c:autoTitleDeleted val="1"/>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="2400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" sz="2400">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+              </a:rPr>
+              <a:t>Register Tile Size Exploration </a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="2400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout>
         <c:manualLayout>
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="9.7908734965821587E-2"/>
-          <c:y val="0.18709052187335146"/>
+          <c:x val="9.3675957172020166E-2"/>
+          <c:y val="0.25408804048377326"/>
           <c:w val="0.87790675507666804"/>
           <c:h val="0.47420312225239836"/>
         </c:manualLayout>
@@ -1351,8 +1406,46 @@
                     <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
                     <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
                   </a:rPr>
-                  <a:t>Tile Configuration</a:t>
+                  <a:t>Register Tile Configuration</a:t>
                 </a:r>
+              </a:p>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr>
+                    <a:solidFill>
+                      <a:schemeClr val="tx1"/>
+                    </a:solidFill>
+                    <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                    <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1600">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1"/>
+                    </a:solidFill>
+                    <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                    <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                  </a:rPr>
+                  <a:t>(N</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1600" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1"/>
+                    </a:solidFill>
+                    <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                    <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                  </a:rPr>
+                  <a:t> = 2880, N_tile = [48, 72, 120, 192])</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US" sz="1600">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1"/>
+                  </a:solidFill>
+                  <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                  <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                </a:endParaRPr>
               </a:p>
             </c:rich>
           </c:tx>
@@ -1360,8 +1453,8 @@
             <c:manualLayout>
               <c:xMode val="edge"/>
               <c:yMode val="edge"/>
-              <c:x val="0.41836538461538464"/>
-              <c:y val="0.82071608604755675"/>
+              <c:x val="0.36228071491063618"/>
+              <c:y val="0.8703438776108321"/>
             </c:manualLayout>
           </c:layout>
           <c:overlay val="0"/>
@@ -1485,8 +1578,8 @@
             <c:manualLayout>
               <c:xMode val="edge"/>
               <c:yMode val="edge"/>
-              <c:x val="2.2615838885523924E-2"/>
-              <c:y val="0.30794943436040723"/>
+              <c:x val="1.8383035453901596E-2"/>
+              <c:y val="0.42953752369043191"/>
             </c:manualLayout>
           </c:layout>
           <c:overlay val="0"/>
@@ -1562,8 +1655,8 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="4.2009063770874794E-2"/>
-          <c:y val="6.2053887184697447E-2"/>
+          <c:x val="4.2009082198058573E-2"/>
+          <c:y val="0.11664445790430042"/>
           <c:w val="0.94395290732889159"/>
           <c:h val="0.10946190969305016"/>
         </c:manualLayout>
@@ -6302,52 +6395,52 @@
   </cols>
   <sheetData>
     <row r="3" spans="4:21" x14ac:dyDescent="0.2">
-      <c r="D3" s="33" t="s">
+      <c r="D3" s="35" t="s">
         <v>29</v>
       </c>
-      <c r="E3" s="33"/>
-      <c r="F3" s="33"/>
-      <c r="G3" s="33"/>
-      <c r="H3" s="33"/>
-      <c r="I3" s="33"/>
-      <c r="J3" s="33"/>
-      <c r="K3" s="33"/>
-      <c r="L3" s="33"/>
-      <c r="M3" s="33"/>
-      <c r="N3" s="33"/>
-      <c r="O3" s="33"/>
-      <c r="P3" s="33"/>
-      <c r="Q3" s="33"/>
-      <c r="R3" s="33"/>
-      <c r="S3" s="33"/>
-      <c r="T3" s="33"/>
-      <c r="U3" s="33"/>
+      <c r="E3" s="35"/>
+      <c r="F3" s="35"/>
+      <c r="G3" s="35"/>
+      <c r="H3" s="35"/>
+      <c r="I3" s="35"/>
+      <c r="J3" s="35"/>
+      <c r="K3" s="35"/>
+      <c r="L3" s="35"/>
+      <c r="M3" s="35"/>
+      <c r="N3" s="35"/>
+      <c r="O3" s="35"/>
+      <c r="P3" s="35"/>
+      <c r="Q3" s="35"/>
+      <c r="R3" s="35"/>
+      <c r="S3" s="35"/>
+      <c r="T3" s="35"/>
+      <c r="U3" s="35"/>
     </row>
     <row r="4" spans="4:21" x14ac:dyDescent="0.2">
-      <c r="D4" s="33" t="s">
+      <c r="D4" s="35" t="s">
         <v>28</v>
       </c>
-      <c r="E4" s="33"/>
-      <c r="F4" s="33"/>
-      <c r="G4" s="33"/>
-      <c r="H4" s="33"/>
-      <c r="I4" s="33"/>
-      <c r="J4" s="33"/>
-      <c r="K4" s="33" t="s">
+      <c r="E4" s="35"/>
+      <c r="F4" s="35"/>
+      <c r="G4" s="35"/>
+      <c r="H4" s="35"/>
+      <c r="I4" s="35"/>
+      <c r="J4" s="35"/>
+      <c r="K4" s="35" t="s">
         <v>26</v>
       </c>
-      <c r="L4" s="33"/>
-      <c r="M4" s="33"/>
-      <c r="N4" s="33"/>
-      <c r="O4" s="33"/>
+      <c r="L4" s="35"/>
+      <c r="M4" s="35"/>
+      <c r="N4" s="35"/>
+      <c r="O4" s="35"/>
       <c r="P4" s="24"/>
-      <c r="Q4" s="33" t="s">
+      <c r="Q4" s="35" t="s">
         <v>27</v>
       </c>
-      <c r="R4" s="33"/>
-      <c r="S4" s="33"/>
-      <c r="T4" s="33"/>
-      <c r="U4" s="33"/>
+      <c r="R4" s="35"/>
+      <c r="S4" s="35"/>
+      <c r="T4" s="35"/>
+      <c r="U4" s="35"/>
     </row>
     <row r="5" spans="4:21" x14ac:dyDescent="0.2">
       <c r="D5" s="1" t="s">
@@ -7106,52 +7199,52 @@
       </c>
     </row>
     <row r="27" spans="4:21" x14ac:dyDescent="0.2">
-      <c r="D27" s="33" t="s">
+      <c r="D27" s="35" t="s">
         <v>30</v>
       </c>
-      <c r="E27" s="33"/>
-      <c r="F27" s="33"/>
-      <c r="G27" s="33"/>
-      <c r="H27" s="33"/>
-      <c r="I27" s="33"/>
-      <c r="J27" s="33"/>
-      <c r="K27" s="33"/>
-      <c r="L27" s="33"/>
-      <c r="M27" s="33"/>
-      <c r="N27" s="33"/>
-      <c r="O27" s="33"/>
-      <c r="P27" s="33"/>
-      <c r="Q27" s="33"/>
-      <c r="R27" s="33"/>
-      <c r="S27" s="33"/>
-      <c r="T27" s="33"/>
-      <c r="U27" s="33"/>
+      <c r="E27" s="35"/>
+      <c r="F27" s="35"/>
+      <c r="G27" s="35"/>
+      <c r="H27" s="35"/>
+      <c r="I27" s="35"/>
+      <c r="J27" s="35"/>
+      <c r="K27" s="35"/>
+      <c r="L27" s="35"/>
+      <c r="M27" s="35"/>
+      <c r="N27" s="35"/>
+      <c r="O27" s="35"/>
+      <c r="P27" s="35"/>
+      <c r="Q27" s="35"/>
+      <c r="R27" s="35"/>
+      <c r="S27" s="35"/>
+      <c r="T27" s="35"/>
+      <c r="U27" s="35"/>
     </row>
     <row r="28" spans="4:21" x14ac:dyDescent="0.2">
-      <c r="D28" s="33" t="s">
+      <c r="D28" s="35" t="s">
         <v>28</v>
       </c>
-      <c r="E28" s="33"/>
-      <c r="F28" s="33"/>
-      <c r="G28" s="33"/>
-      <c r="H28" s="33"/>
-      <c r="I28" s="33"/>
-      <c r="J28" s="33"/>
-      <c r="K28" s="33" t="s">
+      <c r="E28" s="35"/>
+      <c r="F28" s="35"/>
+      <c r="G28" s="35"/>
+      <c r="H28" s="35"/>
+      <c r="I28" s="35"/>
+      <c r="J28" s="35"/>
+      <c r="K28" s="35" t="s">
         <v>26</v>
       </c>
-      <c r="L28" s="33"/>
-      <c r="M28" s="33"/>
-      <c r="N28" s="33"/>
-      <c r="O28" s="33"/>
+      <c r="L28" s="35"/>
+      <c r="M28" s="35"/>
+      <c r="N28" s="35"/>
+      <c r="O28" s="35"/>
       <c r="P28" s="24"/>
-      <c r="Q28" s="33" t="s">
+      <c r="Q28" s="35" t="s">
         <v>27</v>
       </c>
-      <c r="R28" s="33"/>
-      <c r="S28" s="33"/>
-      <c r="T28" s="33"/>
-      <c r="U28" s="33"/>
+      <c r="R28" s="35"/>
+      <c r="S28" s="35"/>
+      <c r="T28" s="35"/>
+      <c r="U28" s="35"/>
     </row>
     <row r="29" spans="4:21" x14ac:dyDescent="0.2">
       <c r="D29" s="1" t="s">
@@ -7910,52 +8003,52 @@
       </c>
     </row>
     <row r="62" spans="4:21" x14ac:dyDescent="0.2">
-      <c r="D62" s="33" t="s">
+      <c r="D62" s="35" t="s">
         <v>32</v>
       </c>
-      <c r="E62" s="33"/>
-      <c r="F62" s="33"/>
-      <c r="G62" s="33"/>
-      <c r="H62" s="33"/>
-      <c r="I62" s="33"/>
-      <c r="J62" s="33"/>
-      <c r="K62" s="33"/>
-      <c r="L62" s="33"/>
-      <c r="M62" s="33"/>
-      <c r="N62" s="33"/>
-      <c r="O62" s="33"/>
-      <c r="P62" s="33"/>
-      <c r="Q62" s="33"/>
-      <c r="R62" s="33"/>
-      <c r="S62" s="33"/>
-      <c r="T62" s="33"/>
-      <c r="U62" s="33"/>
+      <c r="E62" s="35"/>
+      <c r="F62" s="35"/>
+      <c r="G62" s="35"/>
+      <c r="H62" s="35"/>
+      <c r="I62" s="35"/>
+      <c r="J62" s="35"/>
+      <c r="K62" s="35"/>
+      <c r="L62" s="35"/>
+      <c r="M62" s="35"/>
+      <c r="N62" s="35"/>
+      <c r="O62" s="35"/>
+      <c r="P62" s="35"/>
+      <c r="Q62" s="35"/>
+      <c r="R62" s="35"/>
+      <c r="S62" s="35"/>
+      <c r="T62" s="35"/>
+      <c r="U62" s="35"/>
     </row>
     <row r="63" spans="4:21" x14ac:dyDescent="0.2">
-      <c r="D63" s="33" t="s">
+      <c r="D63" s="35" t="s">
         <v>28</v>
       </c>
-      <c r="E63" s="33"/>
-      <c r="F63" s="33"/>
-      <c r="G63" s="33"/>
-      <c r="H63" s="33"/>
-      <c r="I63" s="33"/>
-      <c r="J63" s="33"/>
-      <c r="K63" s="33" t="s">
+      <c r="E63" s="35"/>
+      <c r="F63" s="35"/>
+      <c r="G63" s="35"/>
+      <c r="H63" s="35"/>
+      <c r="I63" s="35"/>
+      <c r="J63" s="35"/>
+      <c r="K63" s="35" t="s">
         <v>26</v>
       </c>
-      <c r="L63" s="33"/>
-      <c r="M63" s="33"/>
-      <c r="N63" s="33"/>
-      <c r="O63" s="33"/>
+      <c r="L63" s="35"/>
+      <c r="M63" s="35"/>
+      <c r="N63" s="35"/>
+      <c r="O63" s="35"/>
       <c r="P63" s="24"/>
-      <c r="Q63" s="33" t="s">
+      <c r="Q63" s="35" t="s">
         <v>27</v>
       </c>
-      <c r="R63" s="33"/>
-      <c r="S63" s="33"/>
-      <c r="T63" s="33"/>
-      <c r="U63" s="33"/>
+      <c r="R63" s="35"/>
+      <c r="S63" s="35"/>
+      <c r="T63" s="35"/>
+      <c r="U63" s="35"/>
     </row>
     <row r="64" spans="4:21" x14ac:dyDescent="0.2">
       <c r="D64" s="1" t="s">
@@ -8713,52 +8806,52 @@
       </c>
     </row>
     <row r="88" spans="4:21" x14ac:dyDescent="0.2">
-      <c r="D88" s="33" t="s">
+      <c r="D88" s="35" t="s">
         <v>31</v>
       </c>
-      <c r="E88" s="33"/>
-      <c r="F88" s="33"/>
-      <c r="G88" s="33"/>
-      <c r="H88" s="33"/>
-      <c r="I88" s="33"/>
-      <c r="J88" s="33"/>
-      <c r="K88" s="33"/>
-      <c r="L88" s="33"/>
-      <c r="M88" s="33"/>
-      <c r="N88" s="33"/>
-      <c r="O88" s="33"/>
-      <c r="P88" s="33"/>
-      <c r="Q88" s="33"/>
-      <c r="R88" s="33"/>
-      <c r="S88" s="33"/>
-      <c r="T88" s="33"/>
-      <c r="U88" s="33"/>
+      <c r="E88" s="35"/>
+      <c r="F88" s="35"/>
+      <c r="G88" s="35"/>
+      <c r="H88" s="35"/>
+      <c r="I88" s="35"/>
+      <c r="J88" s="35"/>
+      <c r="K88" s="35"/>
+      <c r="L88" s="35"/>
+      <c r="M88" s="35"/>
+      <c r="N88" s="35"/>
+      <c r="O88" s="35"/>
+      <c r="P88" s="35"/>
+      <c r="Q88" s="35"/>
+      <c r="R88" s="35"/>
+      <c r="S88" s="35"/>
+      <c r="T88" s="35"/>
+      <c r="U88" s="35"/>
     </row>
     <row r="89" spans="4:21" x14ac:dyDescent="0.2">
-      <c r="D89" s="33" t="s">
+      <c r="D89" s="35" t="s">
         <v>28</v>
       </c>
-      <c r="E89" s="33"/>
-      <c r="F89" s="33"/>
-      <c r="G89" s="33"/>
-      <c r="H89" s="33"/>
-      <c r="I89" s="33"/>
-      <c r="J89" s="33"/>
-      <c r="K89" s="33" t="s">
+      <c r="E89" s="35"/>
+      <c r="F89" s="35"/>
+      <c r="G89" s="35"/>
+      <c r="H89" s="35"/>
+      <c r="I89" s="35"/>
+      <c r="J89" s="35"/>
+      <c r="K89" s="35" t="s">
         <v>26</v>
       </c>
-      <c r="L89" s="33"/>
-      <c r="M89" s="33"/>
-      <c r="N89" s="33"/>
-      <c r="O89" s="33"/>
+      <c r="L89" s="35"/>
+      <c r="M89" s="35"/>
+      <c r="N89" s="35"/>
+      <c r="O89" s="35"/>
       <c r="P89" s="24"/>
-      <c r="Q89" s="33" t="s">
+      <c r="Q89" s="35" t="s">
         <v>27</v>
       </c>
-      <c r="R89" s="33"/>
-      <c r="S89" s="33"/>
-      <c r="T89" s="33"/>
-      <c r="U89" s="33"/>
+      <c r="R89" s="35"/>
+      <c r="S89" s="35"/>
+      <c r="T89" s="35"/>
+      <c r="U89" s="35"/>
     </row>
     <row r="90" spans="4:21" x14ac:dyDescent="0.2">
       <c r="D90" s="1" t="s">
@@ -9559,52 +9652,52 @@
   </cols>
   <sheetData>
     <row r="3" spans="4:21" x14ac:dyDescent="0.2">
-      <c r="D3" s="33" t="s">
+      <c r="D3" s="35" t="s">
         <v>29</v>
       </c>
-      <c r="E3" s="33"/>
-      <c r="F3" s="33"/>
-      <c r="G3" s="33"/>
-      <c r="H3" s="33"/>
-      <c r="I3" s="33"/>
-      <c r="J3" s="33"/>
-      <c r="K3" s="33"/>
-      <c r="L3" s="33"/>
-      <c r="M3" s="33"/>
-      <c r="N3" s="33"/>
-      <c r="O3" s="33"/>
-      <c r="P3" s="33"/>
-      <c r="Q3" s="33"/>
-      <c r="R3" s="33"/>
-      <c r="S3" s="33"/>
-      <c r="T3" s="33"/>
-      <c r="U3" s="33"/>
+      <c r="E3" s="35"/>
+      <c r="F3" s="35"/>
+      <c r="G3" s="35"/>
+      <c r="H3" s="35"/>
+      <c r="I3" s="35"/>
+      <c r="J3" s="35"/>
+      <c r="K3" s="35"/>
+      <c r="L3" s="35"/>
+      <c r="M3" s="35"/>
+      <c r="N3" s="35"/>
+      <c r="O3" s="35"/>
+      <c r="P3" s="35"/>
+      <c r="Q3" s="35"/>
+      <c r="R3" s="35"/>
+      <c r="S3" s="35"/>
+      <c r="T3" s="35"/>
+      <c r="U3" s="35"/>
     </row>
     <row r="4" spans="4:21" x14ac:dyDescent="0.2">
-      <c r="D4" s="33" t="s">
+      <c r="D4" s="35" t="s">
         <v>28</v>
       </c>
-      <c r="E4" s="33"/>
-      <c r="F4" s="33"/>
-      <c r="G4" s="33"/>
-      <c r="H4" s="33"/>
-      <c r="I4" s="33"/>
-      <c r="J4" s="33"/>
-      <c r="K4" s="33" t="s">
+      <c r="E4" s="35"/>
+      <c r="F4" s="35"/>
+      <c r="G4" s="35"/>
+      <c r="H4" s="35"/>
+      <c r="I4" s="35"/>
+      <c r="J4" s="35"/>
+      <c r="K4" s="35" t="s">
         <v>26</v>
       </c>
-      <c r="L4" s="33"/>
-      <c r="M4" s="33"/>
-      <c r="N4" s="33"/>
-      <c r="O4" s="33"/>
+      <c r="L4" s="35"/>
+      <c r="M4" s="35"/>
+      <c r="N4" s="35"/>
+      <c r="O4" s="35"/>
       <c r="P4" s="24"/>
-      <c r="Q4" s="33" t="s">
+      <c r="Q4" s="35" t="s">
         <v>27</v>
       </c>
-      <c r="R4" s="33"/>
-      <c r="S4" s="33"/>
-      <c r="T4" s="33"/>
-      <c r="U4" s="33"/>
+      <c r="R4" s="35"/>
+      <c r="S4" s="35"/>
+      <c r="T4" s="35"/>
+      <c r="U4" s="35"/>
     </row>
     <row r="5" spans="4:21" x14ac:dyDescent="0.2">
       <c r="D5" s="1" t="s">
@@ -10378,52 +10471,52 @@
       </c>
     </row>
     <row r="22" spans="4:21" x14ac:dyDescent="0.2">
-      <c r="D22" s="33" t="s">
+      <c r="D22" s="35" t="s">
         <v>30</v>
       </c>
-      <c r="E22" s="33"/>
-      <c r="F22" s="33"/>
-      <c r="G22" s="33"/>
-      <c r="H22" s="33"/>
-      <c r="I22" s="33"/>
-      <c r="J22" s="33"/>
-      <c r="K22" s="33"/>
-      <c r="L22" s="33"/>
-      <c r="M22" s="33"/>
-      <c r="N22" s="33"/>
-      <c r="O22" s="33"/>
-      <c r="P22" s="33"/>
-      <c r="Q22" s="33"/>
-      <c r="R22" s="33"/>
-      <c r="S22" s="33"/>
-      <c r="T22" s="33"/>
-      <c r="U22" s="33"/>
+      <c r="E22" s="35"/>
+      <c r="F22" s="35"/>
+      <c r="G22" s="35"/>
+      <c r="H22" s="35"/>
+      <c r="I22" s="35"/>
+      <c r="J22" s="35"/>
+      <c r="K22" s="35"/>
+      <c r="L22" s="35"/>
+      <c r="M22" s="35"/>
+      <c r="N22" s="35"/>
+      <c r="O22" s="35"/>
+      <c r="P22" s="35"/>
+      <c r="Q22" s="35"/>
+      <c r="R22" s="35"/>
+      <c r="S22" s="35"/>
+      <c r="T22" s="35"/>
+      <c r="U22" s="35"/>
     </row>
     <row r="23" spans="4:21" x14ac:dyDescent="0.2">
-      <c r="D23" s="33" t="s">
+      <c r="D23" s="35" t="s">
         <v>28</v>
       </c>
-      <c r="E23" s="33"/>
-      <c r="F23" s="33"/>
-      <c r="G23" s="33"/>
-      <c r="H23" s="33"/>
-      <c r="I23" s="33"/>
-      <c r="J23" s="33"/>
-      <c r="K23" s="33" t="s">
+      <c r="E23" s="35"/>
+      <c r="F23" s="35"/>
+      <c r="G23" s="35"/>
+      <c r="H23" s="35"/>
+      <c r="I23" s="35"/>
+      <c r="J23" s="35"/>
+      <c r="K23" s="35" t="s">
         <v>26</v>
       </c>
-      <c r="L23" s="33"/>
-      <c r="M23" s="33"/>
-      <c r="N23" s="33"/>
-      <c r="O23" s="33"/>
+      <c r="L23" s="35"/>
+      <c r="M23" s="35"/>
+      <c r="N23" s="35"/>
+      <c r="O23" s="35"/>
       <c r="P23" s="24"/>
-      <c r="Q23" s="33" t="s">
+      <c r="Q23" s="35" t="s">
         <v>27</v>
       </c>
-      <c r="R23" s="33"/>
-      <c r="S23" s="33"/>
-      <c r="T23" s="33"/>
-      <c r="U23" s="33"/>
+      <c r="R23" s="35"/>
+      <c r="S23" s="35"/>
+      <c r="T23" s="35"/>
+      <c r="U23" s="35"/>
     </row>
     <row r="24" spans="4:21" x14ac:dyDescent="0.2">
       <c r="D24" s="1" t="s">
@@ -11197,52 +11290,52 @@
       </c>
     </row>
     <row r="43" spans="4:21" x14ac:dyDescent="0.2">
-      <c r="D43" s="33" t="s">
+      <c r="D43" s="35" t="s">
         <v>32</v>
       </c>
-      <c r="E43" s="33"/>
-      <c r="F43" s="33"/>
-      <c r="G43" s="33"/>
-      <c r="H43" s="33"/>
-      <c r="I43" s="33"/>
-      <c r="J43" s="33"/>
-      <c r="K43" s="33"/>
-      <c r="L43" s="33"/>
-      <c r="M43" s="33"/>
-      <c r="N43" s="33"/>
-      <c r="O43" s="33"/>
-      <c r="P43" s="33"/>
-      <c r="Q43" s="33"/>
-      <c r="R43" s="33"/>
-      <c r="S43" s="33"/>
-      <c r="T43" s="33"/>
-      <c r="U43" s="33"/>
+      <c r="E43" s="35"/>
+      <c r="F43" s="35"/>
+      <c r="G43" s="35"/>
+      <c r="H43" s="35"/>
+      <c r="I43" s="35"/>
+      <c r="J43" s="35"/>
+      <c r="K43" s="35"/>
+      <c r="L43" s="35"/>
+      <c r="M43" s="35"/>
+      <c r="N43" s="35"/>
+      <c r="O43" s="35"/>
+      <c r="P43" s="35"/>
+      <c r="Q43" s="35"/>
+      <c r="R43" s="35"/>
+      <c r="S43" s="35"/>
+      <c r="T43" s="35"/>
+      <c r="U43" s="35"/>
     </row>
     <row r="44" spans="4:21" x14ac:dyDescent="0.2">
-      <c r="D44" s="33" t="s">
+      <c r="D44" s="35" t="s">
         <v>28</v>
       </c>
-      <c r="E44" s="33"/>
-      <c r="F44" s="33"/>
-      <c r="G44" s="33"/>
-      <c r="H44" s="33"/>
-      <c r="I44" s="33"/>
-      <c r="J44" s="33"/>
-      <c r="K44" s="33" t="s">
+      <c r="E44" s="35"/>
+      <c r="F44" s="35"/>
+      <c r="G44" s="35"/>
+      <c r="H44" s="35"/>
+      <c r="I44" s="35"/>
+      <c r="J44" s="35"/>
+      <c r="K44" s="35" t="s">
         <v>26</v>
       </c>
-      <c r="L44" s="33"/>
-      <c r="M44" s="33"/>
-      <c r="N44" s="33"/>
-      <c r="O44" s="33"/>
+      <c r="L44" s="35"/>
+      <c r="M44" s="35"/>
+      <c r="N44" s="35"/>
+      <c r="O44" s="35"/>
       <c r="P44" s="24"/>
-      <c r="Q44" s="33" t="s">
+      <c r="Q44" s="35" t="s">
         <v>27</v>
       </c>
-      <c r="R44" s="33"/>
-      <c r="S44" s="33"/>
-      <c r="T44" s="33"/>
-      <c r="U44" s="33"/>
+      <c r="R44" s="35"/>
+      <c r="S44" s="35"/>
+      <c r="T44" s="35"/>
+      <c r="U44" s="35"/>
     </row>
     <row r="45" spans="4:21" x14ac:dyDescent="0.2">
       <c r="D45" s="1" t="s">
@@ -12016,52 +12109,52 @@
       </c>
     </row>
     <row r="62" spans="4:21" x14ac:dyDescent="0.2">
-      <c r="D62" s="33" t="s">
+      <c r="D62" s="35" t="s">
         <v>31</v>
       </c>
-      <c r="E62" s="33"/>
-      <c r="F62" s="33"/>
-      <c r="G62" s="33"/>
-      <c r="H62" s="33"/>
-      <c r="I62" s="33"/>
-      <c r="J62" s="33"/>
-      <c r="K62" s="33"/>
-      <c r="L62" s="33"/>
-      <c r="M62" s="33"/>
-      <c r="N62" s="33"/>
-      <c r="O62" s="33"/>
-      <c r="P62" s="33"/>
-      <c r="Q62" s="33"/>
-      <c r="R62" s="33"/>
-      <c r="S62" s="33"/>
-      <c r="T62" s="33"/>
-      <c r="U62" s="33"/>
+      <c r="E62" s="35"/>
+      <c r="F62" s="35"/>
+      <c r="G62" s="35"/>
+      <c r="H62" s="35"/>
+      <c r="I62" s="35"/>
+      <c r="J62" s="35"/>
+      <c r="K62" s="35"/>
+      <c r="L62" s="35"/>
+      <c r="M62" s="35"/>
+      <c r="N62" s="35"/>
+      <c r="O62" s="35"/>
+      <c r="P62" s="35"/>
+      <c r="Q62" s="35"/>
+      <c r="R62" s="35"/>
+      <c r="S62" s="35"/>
+      <c r="T62" s="35"/>
+      <c r="U62" s="35"/>
     </row>
     <row r="63" spans="4:21" x14ac:dyDescent="0.2">
-      <c r="D63" s="33" t="s">
+      <c r="D63" s="35" t="s">
         <v>28</v>
       </c>
-      <c r="E63" s="33"/>
-      <c r="F63" s="33"/>
-      <c r="G63" s="33"/>
-      <c r="H63" s="33"/>
-      <c r="I63" s="33"/>
-      <c r="J63" s="33"/>
-      <c r="K63" s="33" t="s">
+      <c r="E63" s="35"/>
+      <c r="F63" s="35"/>
+      <c r="G63" s="35"/>
+      <c r="H63" s="35"/>
+      <c r="I63" s="35"/>
+      <c r="J63" s="35"/>
+      <c r="K63" s="35" t="s">
         <v>26</v>
       </c>
-      <c r="L63" s="33"/>
-      <c r="M63" s="33"/>
-      <c r="N63" s="33"/>
-      <c r="O63" s="33"/>
+      <c r="L63" s="35"/>
+      <c r="M63" s="35"/>
+      <c r="N63" s="35"/>
+      <c r="O63" s="35"/>
       <c r="P63" s="24"/>
-      <c r="Q63" s="33" t="s">
+      <c r="Q63" s="35" t="s">
         <v>27</v>
       </c>
-      <c r="R63" s="33"/>
-      <c r="S63" s="33"/>
-      <c r="T63" s="33"/>
-      <c r="U63" s="33"/>
+      <c r="R63" s="35"/>
+      <c r="S63" s="35"/>
+      <c r="T63" s="35"/>
+      <c r="U63" s="35"/>
     </row>
     <row r="64" spans="4:21" x14ac:dyDescent="0.2">
       <c r="D64" s="1" t="s">
@@ -12861,8 +12954,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{77F72B3B-E54E-EC40-B8E4-E1260699909C}">
   <dimension ref="D3:L77"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B8" workbookViewId="0">
-      <selection activeCell="V74" sqref="V74"/>
+    <sheetView topLeftCell="A23" workbookViewId="0">
+      <selection activeCell="J6" sqref="J6:L18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -12878,29 +12971,29 @@
   </cols>
   <sheetData>
     <row r="3" spans="4:12" x14ac:dyDescent="0.2">
-      <c r="D3" s="33" t="s">
+      <c r="D3" s="35" t="s">
         <v>29</v>
       </c>
-      <c r="E3" s="33"/>
-      <c r="F3" s="33"/>
-      <c r="G3" s="33"/>
-      <c r="H3" s="33"/>
-      <c r="I3" s="33"/>
-      <c r="J3" s="33"/>
-      <c r="K3" s="33"/>
-      <c r="L3" s="33"/>
+      <c r="E3" s="35"/>
+      <c r="F3" s="35"/>
+      <c r="G3" s="35"/>
+      <c r="H3" s="35"/>
+      <c r="I3" s="35"/>
+      <c r="J3" s="35"/>
+      <c r="K3" s="35"/>
+      <c r="L3" s="35"/>
     </row>
     <row r="4" spans="4:12" x14ac:dyDescent="0.2">
-      <c r="D4" s="33" t="s">
+      <c r="D4" s="35" t="s">
         <v>28</v>
       </c>
-      <c r="E4" s="33"/>
-      <c r="F4" s="33"/>
-      <c r="G4" s="33"/>
-      <c r="H4" s="33"/>
-      <c r="I4" s="33"/>
-      <c r="J4" s="33"/>
-      <c r="K4" s="33"/>
+      <c r="E4" s="35"/>
+      <c r="F4" s="35"/>
+      <c r="G4" s="35"/>
+      <c r="H4" s="35"/>
+      <c r="I4" s="35"/>
+      <c r="J4" s="35"/>
+      <c r="K4" s="35"/>
       <c r="L4" s="24"/>
     </row>
     <row r="5" spans="4:12" x14ac:dyDescent="0.2">
@@ -12951,7 +13044,7 @@
       <c r="I6" s="22">
         <v>48</v>
       </c>
-      <c r="J6" s="34">
+      <c r="J6" s="36">
         <v>48</v>
       </c>
       <c r="K6" s="22" t="s">
@@ -12980,7 +13073,7 @@
       <c r="I7" s="22">
         <v>48</v>
       </c>
-      <c r="J7" s="35"/>
+      <c r="J7" s="37"/>
       <c r="K7" s="21" t="s">
         <v>2</v>
       </c>
@@ -13007,7 +13100,7 @@
       <c r="I8" s="22">
         <v>48</v>
       </c>
-      <c r="J8" s="35"/>
+      <c r="J8" s="37"/>
       <c r="K8" s="21" t="s">
         <v>13</v>
       </c>
@@ -13034,7 +13127,7 @@
       <c r="I9" s="22">
         <v>48</v>
       </c>
-      <c r="J9" s="36"/>
+      <c r="J9" s="38"/>
       <c r="K9" s="21" t="s">
         <v>11</v>
       </c>
@@ -13061,7 +13154,7 @@
       <c r="I10" s="22">
         <v>72</v>
       </c>
-      <c r="J10" s="34">
+      <c r="J10" s="36">
         <v>72</v>
       </c>
       <c r="K10" s="22" t="s">
@@ -13090,7 +13183,7 @@
       <c r="I11" s="22">
         <v>72</v>
       </c>
-      <c r="J11" s="36"/>
+      <c r="J11" s="38"/>
       <c r="K11" s="21" t="s">
         <v>2</v>
       </c>
@@ -13117,7 +13210,7 @@
       <c r="I12" s="25">
         <v>120</v>
       </c>
-      <c r="J12" s="37">
+      <c r="J12" s="39">
         <v>120</v>
       </c>
       <c r="K12" s="25" t="s">
@@ -13146,7 +13239,7 @@
       <c r="I13" s="25">
         <v>120</v>
       </c>
-      <c r="J13" s="38"/>
+      <c r="J13" s="40"/>
       <c r="K13" s="25" t="s">
         <v>2</v>
       </c>
@@ -13173,7 +13266,7 @@
       <c r="I14" s="25">
         <v>192</v>
       </c>
-      <c r="J14" s="37">
+      <c r="J14" s="39">
         <v>192</v>
       </c>
       <c r="K14" s="25" t="s">
@@ -13202,7 +13295,7 @@
       <c r="I15" s="25">
         <v>192</v>
       </c>
-      <c r="J15" s="39"/>
+      <c r="J15" s="41"/>
       <c r="K15" s="25" t="s">
         <v>1</v>
       </c>
@@ -13229,7 +13322,7 @@
       <c r="I16" s="25">
         <v>192</v>
       </c>
-      <c r="J16" s="39"/>
+      <c r="J16" s="41"/>
       <c r="K16" s="25" t="s">
         <v>2</v>
       </c>
@@ -13256,7 +13349,7 @@
       <c r="I17" s="25">
         <v>192</v>
       </c>
-      <c r="J17" s="39"/>
+      <c r="J17" s="41"/>
       <c r="K17" s="25" t="s">
         <v>13</v>
       </c>
@@ -13283,7 +13376,7 @@
       <c r="I18" s="25">
         <v>192</v>
       </c>
-      <c r="J18" s="38"/>
+      <c r="J18" s="40"/>
       <c r="K18" s="25" t="s">
         <v>11</v>
       </c>
@@ -13292,29 +13385,29 @@
       </c>
     </row>
     <row r="21" spans="4:12" x14ac:dyDescent="0.2">
-      <c r="D21" s="33" t="s">
+      <c r="D21" s="35" t="s">
         <v>30</v>
       </c>
-      <c r="E21" s="33"/>
-      <c r="F21" s="33"/>
-      <c r="G21" s="33"/>
-      <c r="H21" s="33"/>
-      <c r="I21" s="33"/>
-      <c r="J21" s="33"/>
-      <c r="K21" s="33"/>
-      <c r="L21" s="33"/>
+      <c r="E21" s="35"/>
+      <c r="F21" s="35"/>
+      <c r="G21" s="35"/>
+      <c r="H21" s="35"/>
+      <c r="I21" s="35"/>
+      <c r="J21" s="35"/>
+      <c r="K21" s="35"/>
+      <c r="L21" s="35"/>
     </row>
     <row r="22" spans="4:12" x14ac:dyDescent="0.2">
-      <c r="D22" s="33" t="s">
+      <c r="D22" s="35" t="s">
         <v>28</v>
       </c>
-      <c r="E22" s="33"/>
-      <c r="F22" s="33"/>
-      <c r="G22" s="33"/>
-      <c r="H22" s="33"/>
-      <c r="I22" s="33"/>
-      <c r="J22" s="33"/>
-      <c r="K22" s="33"/>
+      <c r="E22" s="35"/>
+      <c r="F22" s="35"/>
+      <c r="G22" s="35"/>
+      <c r="H22" s="35"/>
+      <c r="I22" s="35"/>
+      <c r="J22" s="35"/>
+      <c r="K22" s="35"/>
       <c r="L22" s="24"/>
     </row>
     <row r="23" spans="4:12" x14ac:dyDescent="0.2">
@@ -13365,7 +13458,7 @@
       <c r="I24" s="22">
         <v>48</v>
       </c>
-      <c r="J24" s="34">
+      <c r="J24" s="36">
         <v>48</v>
       </c>
       <c r="K24" s="22" t="s">
@@ -13394,7 +13487,7 @@
       <c r="I25" s="22">
         <v>48</v>
       </c>
-      <c r="J25" s="35"/>
+      <c r="J25" s="37"/>
       <c r="K25" s="21" t="s">
         <v>2</v>
       </c>
@@ -13421,7 +13514,7 @@
       <c r="I26" s="22">
         <v>48</v>
       </c>
-      <c r="J26" s="35"/>
+      <c r="J26" s="37"/>
       <c r="K26" s="21" t="s">
         <v>13</v>
       </c>
@@ -13448,7 +13541,7 @@
       <c r="I27" s="22">
         <v>48</v>
       </c>
-      <c r="J27" s="36"/>
+      <c r="J27" s="38"/>
       <c r="K27" s="21" t="s">
         <v>11</v>
       </c>
@@ -13475,7 +13568,7 @@
       <c r="I28" s="22">
         <v>72</v>
       </c>
-      <c r="J28" s="34">
+      <c r="J28" s="36">
         <v>72</v>
       </c>
       <c r="K28" s="22" t="s">
@@ -13504,7 +13597,7 @@
       <c r="I29" s="22">
         <v>72</v>
       </c>
-      <c r="J29" s="36"/>
+      <c r="J29" s="38"/>
       <c r="K29" s="21" t="s">
         <v>2</v>
       </c>
@@ -13531,7 +13624,7 @@
       <c r="I30" s="25">
         <v>120</v>
       </c>
-      <c r="J30" s="37">
+      <c r="J30" s="39">
         <v>120</v>
       </c>
       <c r="K30" s="25" t="s">
@@ -13560,7 +13653,7 @@
       <c r="I31" s="25">
         <v>120</v>
       </c>
-      <c r="J31" s="38"/>
+      <c r="J31" s="40"/>
       <c r="K31" s="25" t="s">
         <v>2</v>
       </c>
@@ -13587,7 +13680,7 @@
       <c r="I32" s="25">
         <v>192</v>
       </c>
-      <c r="J32" s="37">
+      <c r="J32" s="39">
         <v>192</v>
       </c>
       <c r="K32" s="25" t="s">
@@ -13616,7 +13709,7 @@
       <c r="I33" s="25">
         <v>192</v>
       </c>
-      <c r="J33" s="39"/>
+      <c r="J33" s="41"/>
       <c r="K33" s="25" t="s">
         <v>1</v>
       </c>
@@ -13643,7 +13736,7 @@
       <c r="I34" s="25">
         <v>192</v>
       </c>
-      <c r="J34" s="39"/>
+      <c r="J34" s="41"/>
       <c r="K34" s="25" t="s">
         <v>2</v>
       </c>
@@ -13670,7 +13763,7 @@
       <c r="I35" s="25">
         <v>192</v>
       </c>
-      <c r="J35" s="39"/>
+      <c r="J35" s="41"/>
       <c r="K35" s="25" t="s">
         <v>13</v>
       </c>
@@ -13697,7 +13790,7 @@
       <c r="I36" s="25">
         <v>192</v>
       </c>
-      <c r="J36" s="38"/>
+      <c r="J36" s="40"/>
       <c r="K36" s="25" t="s">
         <v>11</v>
       </c>
@@ -13709,42 +13802,42 @@
       <c r="J37" t="s">
         <v>37</v>
       </c>
-      <c r="K37" s="40" t="s">
+      <c r="K37" s="33" t="s">
         <v>39</v>
       </c>
-      <c r="L37" s="41">
+      <c r="L37" s="34">
         <v>80</v>
       </c>
     </row>
     <row r="38" spans="4:12" x14ac:dyDescent="0.2">
-      <c r="K38" s="40" t="s">
+      <c r="K38" s="33" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="42" spans="4:12" x14ac:dyDescent="0.2">
-      <c r="D42" s="33" t="s">
+      <c r="D42" s="35" t="s">
         <v>34</v>
       </c>
-      <c r="E42" s="33"/>
-      <c r="F42" s="33"/>
-      <c r="G42" s="33"/>
-      <c r="H42" s="33"/>
-      <c r="I42" s="33"/>
-      <c r="J42" s="33"/>
-      <c r="K42" s="33"/>
-      <c r="L42" s="33"/>
+      <c r="E42" s="35"/>
+      <c r="F42" s="35"/>
+      <c r="G42" s="35"/>
+      <c r="H42" s="35"/>
+      <c r="I42" s="35"/>
+      <c r="J42" s="35"/>
+      <c r="K42" s="35"/>
+      <c r="L42" s="35"/>
     </row>
     <row r="43" spans="4:12" x14ac:dyDescent="0.2">
-      <c r="D43" s="33" t="s">
+      <c r="D43" s="35" t="s">
         <v>28</v>
       </c>
-      <c r="E43" s="33"/>
-      <c r="F43" s="33"/>
-      <c r="G43" s="33"/>
-      <c r="H43" s="33"/>
-      <c r="I43" s="33"/>
-      <c r="J43" s="33"/>
-      <c r="K43" s="33"/>
+      <c r="E43" s="35"/>
+      <c r="F43" s="35"/>
+      <c r="G43" s="35"/>
+      <c r="H43" s="35"/>
+      <c r="I43" s="35"/>
+      <c r="J43" s="35"/>
+      <c r="K43" s="35"/>
       <c r="L43" s="24"/>
     </row>
     <row r="44" spans="4:12" x14ac:dyDescent="0.2">
@@ -13795,7 +13888,7 @@
       <c r="I45" s="22">
         <v>48</v>
       </c>
-      <c r="J45" s="34">
+      <c r="J45" s="36">
         <v>48</v>
       </c>
       <c r="K45" s="22" t="s">
@@ -13824,7 +13917,7 @@
       <c r="I46" s="22">
         <v>48</v>
       </c>
-      <c r="J46" s="35"/>
+      <c r="J46" s="37"/>
       <c r="K46" s="21" t="s">
         <v>2</v>
       </c>
@@ -13851,7 +13944,7 @@
       <c r="I47" s="22">
         <v>48</v>
       </c>
-      <c r="J47" s="35"/>
+      <c r="J47" s="37"/>
       <c r="K47" s="21" t="s">
         <v>13</v>
       </c>
@@ -13878,7 +13971,7 @@
       <c r="I48" s="22">
         <v>48</v>
       </c>
-      <c r="J48" s="36"/>
+      <c r="J48" s="38"/>
       <c r="K48" s="21" t="s">
         <v>11</v>
       </c>
@@ -13905,7 +13998,7 @@
       <c r="I49" s="22">
         <v>72</v>
       </c>
-      <c r="J49" s="34">
+      <c r="J49" s="36">
         <v>72</v>
       </c>
       <c r="K49" s="22" t="s">
@@ -13934,7 +14027,7 @@
       <c r="I50" s="22">
         <v>72</v>
       </c>
-      <c r="J50" s="36"/>
+      <c r="J50" s="38"/>
       <c r="K50" s="21" t="s">
         <v>2</v>
       </c>
@@ -13961,7 +14054,7 @@
       <c r="I51" s="25">
         <v>120</v>
       </c>
-      <c r="J51" s="37">
+      <c r="J51" s="39">
         <v>120</v>
       </c>
       <c r="K51" s="25" t="s">
@@ -13990,7 +14083,7 @@
       <c r="I52" s="25">
         <v>120</v>
       </c>
-      <c r="J52" s="38"/>
+      <c r="J52" s="40"/>
       <c r="K52" s="25" t="s">
         <v>2</v>
       </c>
@@ -14017,7 +14110,7 @@
       <c r="I53" s="25">
         <v>192</v>
       </c>
-      <c r="J53" s="37">
+      <c r="J53" s="39">
         <v>192</v>
       </c>
       <c r="K53" s="25" t="s">
@@ -14046,7 +14139,7 @@
       <c r="I54" s="25">
         <v>192</v>
       </c>
-      <c r="J54" s="39"/>
+      <c r="J54" s="41"/>
       <c r="K54" s="25" t="s">
         <v>1</v>
       </c>
@@ -14073,7 +14166,7 @@
       <c r="I55" s="25">
         <v>192</v>
       </c>
-      <c r="J55" s="39"/>
+      <c r="J55" s="41"/>
       <c r="K55" s="25" t="s">
         <v>2</v>
       </c>
@@ -14100,7 +14193,7 @@
       <c r="I56" s="25">
         <v>192</v>
       </c>
-      <c r="J56" s="39"/>
+      <c r="J56" s="41"/>
       <c r="K56" s="25" t="s">
         <v>13</v>
       </c>
@@ -14127,7 +14220,7 @@
       <c r="I57" s="25">
         <v>192</v>
       </c>
-      <c r="J57" s="38"/>
+      <c r="J57" s="40"/>
       <c r="K57" s="25" t="s">
         <v>11</v>
       </c>
@@ -14136,29 +14229,29 @@
       </c>
     </row>
     <row r="61" spans="4:12" x14ac:dyDescent="0.2">
-      <c r="D61" s="33" t="s">
+      <c r="D61" s="35" t="s">
         <v>35</v>
       </c>
-      <c r="E61" s="33"/>
-      <c r="F61" s="33"/>
-      <c r="G61" s="33"/>
-      <c r="H61" s="33"/>
-      <c r="I61" s="33"/>
-      <c r="J61" s="33"/>
-      <c r="K61" s="33"/>
-      <c r="L61" s="33"/>
+      <c r="E61" s="35"/>
+      <c r="F61" s="35"/>
+      <c r="G61" s="35"/>
+      <c r="H61" s="35"/>
+      <c r="I61" s="35"/>
+      <c r="J61" s="35"/>
+      <c r="K61" s="35"/>
+      <c r="L61" s="35"/>
     </row>
     <row r="62" spans="4:12" x14ac:dyDescent="0.2">
-      <c r="D62" s="33" t="s">
+      <c r="D62" s="35" t="s">
         <v>28</v>
       </c>
-      <c r="E62" s="33"/>
-      <c r="F62" s="33"/>
-      <c r="G62" s="33"/>
-      <c r="H62" s="33"/>
-      <c r="I62" s="33"/>
-      <c r="J62" s="33"/>
-      <c r="K62" s="33"/>
+      <c r="E62" s="35"/>
+      <c r="F62" s="35"/>
+      <c r="G62" s="35"/>
+      <c r="H62" s="35"/>
+      <c r="I62" s="35"/>
+      <c r="J62" s="35"/>
+      <c r="K62" s="35"/>
       <c r="L62" s="24"/>
     </row>
     <row r="63" spans="4:12" x14ac:dyDescent="0.2">
@@ -14209,7 +14302,7 @@
       <c r="I64" s="22">
         <v>48</v>
       </c>
-      <c r="J64" s="34">
+      <c r="J64" s="36">
         <v>48</v>
       </c>
       <c r="K64" s="22" t="s">
@@ -14238,7 +14331,7 @@
       <c r="I65" s="22">
         <v>48</v>
       </c>
-      <c r="J65" s="35"/>
+      <c r="J65" s="37"/>
       <c r="K65" s="21" t="s">
         <v>2</v>
       </c>
@@ -14265,7 +14358,7 @@
       <c r="I66" s="22">
         <v>48</v>
       </c>
-      <c r="J66" s="35"/>
+      <c r="J66" s="37"/>
       <c r="K66" s="21" t="s">
         <v>13</v>
       </c>
@@ -14292,7 +14385,7 @@
       <c r="I67" s="22">
         <v>48</v>
       </c>
-      <c r="J67" s="36"/>
+      <c r="J67" s="38"/>
       <c r="K67" s="21" t="s">
         <v>11</v>
       </c>
@@ -14319,7 +14412,7 @@
       <c r="I68" s="22">
         <v>72</v>
       </c>
-      <c r="J68" s="34">
+      <c r="J68" s="36">
         <v>72</v>
       </c>
       <c r="K68" s="22" t="s">
@@ -14348,7 +14441,7 @@
       <c r="I69" s="22">
         <v>72</v>
       </c>
-      <c r="J69" s="36"/>
+      <c r="J69" s="38"/>
       <c r="K69" s="21" t="s">
         <v>2</v>
       </c>
@@ -14375,7 +14468,7 @@
       <c r="I70" s="25">
         <v>120</v>
       </c>
-      <c r="J70" s="37">
+      <c r="J70" s="39">
         <v>120</v>
       </c>
       <c r="K70" s="25" t="s">
@@ -14404,7 +14497,7 @@
       <c r="I71" s="25">
         <v>120</v>
       </c>
-      <c r="J71" s="38"/>
+      <c r="J71" s="40"/>
       <c r="K71" s="25" t="s">
         <v>2</v>
       </c>
@@ -14431,7 +14524,7 @@
       <c r="I72" s="25">
         <v>192</v>
       </c>
-      <c r="J72" s="37">
+      <c r="J72" s="39">
         <v>192</v>
       </c>
       <c r="K72" s="25" t="s">
@@ -14460,7 +14553,7 @@
       <c r="I73" s="25">
         <v>192</v>
       </c>
-      <c r="J73" s="39"/>
+      <c r="J73" s="41"/>
       <c r="K73" s="25" t="s">
         <v>1</v>
       </c>
@@ -14487,7 +14580,7 @@
       <c r="I74" s="25">
         <v>192</v>
       </c>
-      <c r="J74" s="39"/>
+      <c r="J74" s="41"/>
       <c r="K74" s="25" t="s">
         <v>2</v>
       </c>
@@ -14514,7 +14607,7 @@
       <c r="I75" s="25">
         <v>192</v>
       </c>
-      <c r="J75" s="39"/>
+      <c r="J75" s="41"/>
       <c r="K75" s="25" t="s">
         <v>13</v>
       </c>
@@ -14541,7 +14634,7 @@
       <c r="I76" s="25">
         <v>192</v>
       </c>
-      <c r="J76" s="38"/>
+      <c r="J76" s="40"/>
       <c r="K76" s="25" t="s">
         <v>11</v>
       </c>
@@ -14553,15 +14646,26 @@
       <c r="J77" t="s">
         <v>37</v>
       </c>
-      <c r="K77" s="40" t="s">
+      <c r="K77" s="33" t="s">
         <v>38</v>
       </c>
-      <c r="L77" s="41">
+      <c r="L77" s="34">
         <v>32</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="24">
+    <mergeCell ref="J24:J27"/>
+    <mergeCell ref="J28:J29"/>
+    <mergeCell ref="J30:J31"/>
+    <mergeCell ref="D3:L3"/>
+    <mergeCell ref="D4:K4"/>
+    <mergeCell ref="D21:L21"/>
+    <mergeCell ref="D22:K22"/>
+    <mergeCell ref="J6:J9"/>
+    <mergeCell ref="J10:J11"/>
+    <mergeCell ref="J12:J13"/>
+    <mergeCell ref="J14:J18"/>
     <mergeCell ref="J64:J67"/>
     <mergeCell ref="J68:J69"/>
     <mergeCell ref="J70:J71"/>
@@ -14575,17 +14679,6 @@
     <mergeCell ref="D43:K43"/>
     <mergeCell ref="D61:L61"/>
     <mergeCell ref="D62:K62"/>
-    <mergeCell ref="D3:L3"/>
-    <mergeCell ref="D4:K4"/>
-    <mergeCell ref="D21:L21"/>
-    <mergeCell ref="D22:K22"/>
-    <mergeCell ref="J6:J9"/>
-    <mergeCell ref="J10:J11"/>
-    <mergeCell ref="J12:J13"/>
-    <mergeCell ref="J14:J18"/>
-    <mergeCell ref="J24:J27"/>
-    <mergeCell ref="J28:J29"/>
-    <mergeCell ref="J30:J31"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -15138,7 +15231,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1D6A475-C568-8040-BE9B-325734E81B21}">
   <dimension ref="C9:K23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="K9" sqref="K9"/>
     </sheetView>
   </sheetViews>

</xml_diff>